<commit_message>
Complete disparity paper and supplementary drafts
</commit_message>
<xml_diff>
--- a/Disparity/output/disp_results_summary.xlsx
+++ b/Disparity/output/disp_results_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="18180" windowHeight="9264"/>
+    <workbookView xWindow="480" yWindow="156" windowWidth="18180" windowHeight="9204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,6 +167,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,8 +178,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,22 +543,22 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="9" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -617,19 +617,19 @@
         <v>10</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="3"/>
@@ -681,7 +681,7 @@
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -724,7 +724,7 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="1"/>

</xml_diff>